<commit_message>
Working on making launch_intent results look nice.
</commit_message>
<xml_diff>
--- a/form-files/selects/selects.xlsx
+++ b/form-files/selects/selects.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58" count="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62" count="74">
   <si>
     <t>comments</t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t>callback</t>
+  </si>
+  <si>
+    <t>param.format</t>
+  </si>
+  <si>
+    <t>param.q</t>
   </si>
   <si>
     <t>states</t>
@@ -170,6 +176,12 @@
   </si>
   <si>
     <t>"https://query.yahooapis.com/v1/public/yql?format=json&amp;q=" +  encodeURIComponent("select * from geo.states where place='" + data('state') + "'")</t>
+  </si>
+  <si>
+    <t>odk_values</t>
+  </si>
+  <si>
+    <t>odkquery://table_id/elementKey1/elementKey5/?selection=encodeURIComponent('elementKey2=? and elementKey3&gt;5')&amp;selectionArgs=encodeURIComponent(JSON.stringify([data('state')])</t>
   </si>
   <si>
     <t>setting</t>
@@ -692,27 +704,41 @@
       <c t="s" r="C1">
         <v>45</v>
       </c>
+      <c t="s" r="D1">
+        <v>46</v>
+      </c>
+      <c t="s" r="E1">
+        <v>47</v>
+      </c>
     </row>
     <row r="2">
       <c t="s" r="A2">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c t="s" r="B2">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c t="s" r="C2">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
       <c t="s" r="A3">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c t="s" r="B3">
+        <v>52</v>
+      </c>
+      <c t="s" r="C3">
         <v>50</v>
       </c>
-      <c t="s" r="C3">
-        <v>48</v>
+    </row>
+    <row r="5">
+      <c t="s" r="A5">
+        <v>53</v>
+      </c>
+      <c t="s" r="B5">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -728,25 +754,25 @@
   <sheetData>
     <row r="1">
       <c t="s" s="2" r="A1">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c t="s" s="2" r="B1">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c s="2" r="C1"/>
     </row>
     <row r="2">
       <c t="s" s="2" r="A2">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c t="s" s="2" r="B2">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c s="2" r="C2"/>
     </row>
     <row r="3">
       <c t="s" s="2" r="A3">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -754,10 +780,10 @@
     </row>
     <row r="4">
       <c t="s" r="A4">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c t="s" r="B4">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Adding grid/inline select appearance properties
</commit_message>
<xml_diff>
--- a/form-files/selects/selects.xlsx
+++ b/form-files/selects/selects.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62" count="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73" count="95">
   <si>
     <t>comments</t>
   </si>
@@ -22,6 +22,9 @@
     <t>type</t>
   </si>
   <si>
+    <t>appearance</t>
+  </si>
+  <si>
     <t>condition</t>
   </si>
   <si>
@@ -61,6 +64,9 @@
     <t>select_one birds</t>
   </si>
   <si>
+    <t>grid</t>
+  </si>
+  <si>
     <t>bird</t>
   </si>
   <si>
@@ -85,6 +91,24 @@
     <t>end screen</t>
   </si>
   <si>
+    <t>select_one yes_no</t>
+  </si>
+  <si>
+    <t>inline</t>
+  </si>
+  <si>
+    <t>i1</t>
+  </si>
+  <si>
+    <t>Choose one:</t>
+  </si>
+  <si>
+    <t>i2</t>
+  </si>
+  <si>
+    <t>i3</t>
+  </si>
+  <si>
     <t>list_name</t>
   </si>
   <si>
@@ -148,16 +172,25 @@
     <t>media/jay.png</t>
   </si>
   <si>
+    <t>yes_no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>uri</t>
   </si>
   <si>
     <t>callback</t>
-  </si>
-  <si>
-    <t>param.format</t>
-  </si>
-  <si>
-    <t>param.q</t>
   </si>
   <si>
     <t>states</t>
@@ -181,7 +214,7 @@
     <t>odk_values</t>
   </si>
   <si>
-    <t>odkquery://table_id/elementKey1/elementKey5/?selection=encodeURIComponent('elementKey2=? and elementKey3&gt;5')&amp;selectionArgs=encodeURIComponent(JSON.stringify([data('state')])</t>
+    <t>"content://com.opendatakit.tables.ContentProvider/database_id/table_id/row_id"</t>
   </si>
   <si>
     <t>setting</t>
@@ -415,9 +448,9 @@
   <cols>
     <col max="1" min="1" customWidth="1" width="34.29"/>
     <col max="2" min="2" customWidth="1" width="35.0"/>
-    <col max="3" min="3" customWidth="1" width="38.71"/>
-    <col max="4" min="4" customWidth="1" width="32.71"/>
-    <col max="5" min="5" customWidth="1" width="37.71"/>
+    <col max="4" min="4" customWidth="1" width="38.71"/>
+    <col max="5" min="5" customWidth="1" width="32.71"/>
+    <col max="6" min="6" customWidth="1" width="37.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -436,97 +469,145 @@
       <c t="s" r="E1">
         <v>4</v>
       </c>
+      <c t="s" r="F1">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c t="s" s="12" r="A2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c t="s" r="B2">
-        <v>6</v>
-      </c>
-      <c t="s" r="D2">
         <v>7</v>
       </c>
       <c t="s" r="E2">
         <v>8</v>
+      </c>
+      <c t="s" r="F2">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c s="12" r="A3"/>
       <c t="s" r="B3">
-        <v>9</v>
-      </c>
-      <c t="s" r="D3">
         <v>10</v>
       </c>
       <c t="s" r="E3">
         <v>11</v>
       </c>
+      <c t="s" r="F3">
+        <v>12</v>
+      </c>
     </row>
     <row r="4">
       <c t="s" s="12" r="A4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c t="s" r="B4">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c s="12" r="A5"/>
       <c t="s" r="B5">
-        <v>14</v>
-      </c>
-      <c t="s" r="D5">
         <v>15</v>
       </c>
+      <c t="s" r="C5">
+        <v>16</v>
+      </c>
       <c t="s" r="E5">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c t="s" r="F5">
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c s="12" r="A6"/>
       <c t="s" r="B6">
-        <v>17</v>
-      </c>
-      <c t="s" r="C6">
-        <v>18</v>
-      </c>
-      <c t="s" r="E6">
         <v>19</v>
+      </c>
+      <c t="s" r="D6">
+        <v>20</v>
+      </c>
+      <c t="s" r="F6">
+        <v>21</v>
       </c>
     </row>
     <row r="7">
       <c s="12" r="A7"/>
       <c t="s" r="B7">
-        <v>17</v>
-      </c>
-      <c t="s" r="C7">
-        <v>20</v>
-      </c>
-      <c t="s" r="E7">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c t="s" r="D7">
+        <v>22</v>
+      </c>
+      <c t="s" r="F7">
+        <v>23</v>
       </c>
     </row>
     <row r="8">
       <c s="12" r="A8"/>
       <c t="s" r="B8">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9">
       <c s="12" r="A9"/>
+      <c t="s" r="B9">
+        <v>14</v>
+      </c>
     </row>
     <row r="10">
       <c s="12" r="A10"/>
+      <c t="s" r="B10">
+        <v>25</v>
+      </c>
+      <c t="s" r="C10">
+        <v>26</v>
+      </c>
+      <c t="s" r="E10">
+        <v>27</v>
+      </c>
+      <c t="s" r="F10">
+        <v>28</v>
+      </c>
     </row>
     <row r="11">
       <c s="12" r="A11"/>
+      <c t="s" r="B11">
+        <v>25</v>
+      </c>
+      <c t="s" r="C11">
+        <v>26</v>
+      </c>
+      <c t="s" r="E11">
+        <v>29</v>
+      </c>
+      <c t="s" r="F11">
+        <v>28</v>
+      </c>
     </row>
     <row r="12">
       <c s="12" r="A12"/>
+      <c t="s" r="B12">
+        <v>25</v>
+      </c>
+      <c t="s" r="C12">
+        <v>26</v>
+      </c>
+      <c t="s" r="E12">
+        <v>30</v>
+      </c>
+      <c t="s" r="F12">
+        <v>28</v>
+      </c>
     </row>
     <row r="13">
       <c s="12" r="A13"/>
+      <c t="s" r="B13">
+        <v>24</v>
+      </c>
     </row>
     <row r="14">
       <c s="12" r="A14"/>
@@ -571,112 +652,137 @@
   <sheetData>
     <row r="1">
       <c t="s" r="A1">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c t="s" r="B1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c t="s" r="C1">
-        <v>24</v>
+        <v>32</v>
+      </c>
+      <c t="s" r="D1">
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c t="s" r="A2">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c t="s" r="B2">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c t="s" r="C2">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3">
       <c t="s" r="A3">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c t="s" r="B3">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c t="s" r="C3">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4">
       <c t="s" r="A4">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c t="s" r="B4">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c t="s" r="C4">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5">
       <c t="s" r="A5">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c t="s" r="B5">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c t="s" r="C5">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6">
       <c t="s" r="A6">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c t="s" r="B6">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c t="s" r="C6">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7">
       <c t="s" r="A7">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c t="s" r="B7">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c t="s" r="C7">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8">
       <c t="s" r="A8">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c t="s" r="B8">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c t="s" r="C8">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9">
       <c t="s" r="A9">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c t="s" r="B9">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c t="s" r="C9">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10">
       <c t="s" r="A10">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c t="s" r="B10">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c t="s" r="C10">
-        <v>43</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12">
+      <c t="s" r="A12">
+        <v>52</v>
+      </c>
+      <c t="s" r="B12">
+        <v>53</v>
+      </c>
+      <c t="s" r="D12">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13">
+      <c t="s" r="A13">
+        <v>52</v>
+      </c>
+      <c t="s" r="B13">
+        <v>55</v>
+      </c>
+      <c t="s" r="D13">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -690,55 +796,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="17.14" customHeight="1"/>
   <cols>
-    <col max="2" min="2" customWidth="1" width="39.14"/>
+    <col max="2" min="2" customWidth="1" width="71.29"/>
     <col max="3" min="3" customWidth="1" width="35.14"/>
   </cols>
   <sheetData>
     <row r="1">
       <c t="s" r="A1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c t="s" r="B1">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c t="s" r="C1">
-        <v>45</v>
-      </c>
-      <c t="s" r="D1">
-        <v>46</v>
-      </c>
-      <c t="s" r="E1">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2">
       <c t="s" r="A2">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c t="s" r="B2">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c t="s" r="C2">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3">
       <c t="s" r="A3">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c t="s" r="B3">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c t="s" r="C3">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5">
       <c t="s" r="A5">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c t="s" r="B5">
-        <v>54</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -754,25 +854,25 @@
   <sheetData>
     <row r="1">
       <c t="s" s="2" r="A1">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c t="s" s="2" r="B1">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c s="2" r="C1"/>
     </row>
     <row r="2">
       <c t="s" s="2" r="A2">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c t="s" s="2" r="B2">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c s="2" r="C2"/>
     </row>
     <row r="3">
       <c t="s" s="2" r="A3">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -780,10 +880,10 @@
     </row>
     <row r="4">
       <c t="s" r="A4">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c t="s" r="B4">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Fixing a host of issues with select_one_with_other
</commit_message>
<xml_diff>
--- a/form-files/selects/selects.xlsx
+++ b/form-files/selects/selects.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73" count="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="86" count="111">
   <si>
     <t>comments</t>
   </si>
@@ -109,6 +109,24 @@
     <t>i3</t>
   </si>
   <si>
+    <t>select_one_with_other colors</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>What is your favorite color?</t>
+  </si>
+  <si>
+    <t>selected function with arguement not included in choices.</t>
+  </si>
+  <si>
+    <t>selected(data('color'), 'teal')</t>
+  </si>
+  <si>
+    <t>Teal is a good choice.</t>
+  </si>
+  <si>
     <t>list_name</t>
   </si>
   <si>
@@ -185,6 +203,27 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>colors</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>Blue</t>
   </si>
   <si>
     <t>uri</t>
@@ -611,9 +650,29 @@
     </row>
     <row r="14">
       <c s="12" r="A14"/>
+      <c t="s" r="B14">
+        <v>31</v>
+      </c>
+      <c t="s" r="E14">
+        <v>32</v>
+      </c>
+      <c t="s" r="F14">
+        <v>33</v>
+      </c>
     </row>
     <row r="15">
-      <c s="12" r="A15"/>
+      <c t="s" s="12" r="A15">
+        <v>34</v>
+      </c>
+      <c t="s" r="B15">
+        <v>19</v>
+      </c>
+      <c t="s" r="D15">
+        <v>35</v>
+      </c>
+      <c t="s" r="F15">
+        <v>36</v>
+      </c>
     </row>
     <row r="16">
       <c s="12" r="A16"/>
@@ -652,13 +711,13 @@
   <sheetData>
     <row r="1">
       <c t="s" r="A1">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c t="s" r="B1">
         <v>4</v>
       </c>
       <c t="s" r="C1">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c t="s" r="D1">
         <v>5</v>
@@ -666,123 +725,156 @@
     </row>
     <row r="2">
       <c t="s" r="A2">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c t="s" r="B2">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c t="s" r="C2">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3">
       <c t="s" r="A3">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c t="s" r="B3">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c t="s" r="C3">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4">
       <c t="s" r="A4">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c t="s" r="B4">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c t="s" r="C4">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5">
       <c t="s" r="A5">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c t="s" r="B5">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c t="s" r="C5">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6">
       <c t="s" r="A6">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c t="s" r="B6">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c t="s" r="C6">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7">
       <c t="s" r="A7">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c t="s" r="B7">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c t="s" r="C7">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8">
       <c t="s" r="A8">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c t="s" r="B8">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c t="s" r="C8">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9">
       <c t="s" r="A9">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c t="s" r="B9">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c t="s" r="C9">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10">
       <c t="s" r="A10">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c t="s" r="B10">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c t="s" r="C10">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12">
       <c t="s" r="A12">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c t="s" r="B12">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c t="s" r="D12">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13">
       <c t="s" r="A13">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c t="s" r="B13">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c t="s" r="D13">
-        <v>56</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15">
+      <c t="s" r="A15">
+        <v>63</v>
+      </c>
+      <c t="s" r="B15">
+        <v>64</v>
+      </c>
+      <c t="s" r="D15">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16">
+      <c t="s" r="A16">
+        <v>63</v>
+      </c>
+      <c t="s" r="B16">
+        <v>66</v>
+      </c>
+      <c t="s" r="D16">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17">
+      <c t="s" r="A17">
+        <v>63</v>
+      </c>
+      <c t="s" r="B17">
+        <v>68</v>
+      </c>
+      <c t="s" r="D17">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -805,40 +897,40 @@
         <v>4</v>
       </c>
       <c t="s" r="B1">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c t="s" r="C1">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2">
       <c t="s" r="A2">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c t="s" r="B2">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c t="s" r="C2">
-        <v>61</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3">
       <c t="s" r="A3">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c t="s" r="B3">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c t="s" r="C3">
-        <v>61</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5">
       <c t="s" r="A5">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c t="s" r="B5">
-        <v>65</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -854,25 +946,25 @@
   <sheetData>
     <row r="1">
       <c t="s" s="2" r="A1">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c t="s" s="2" r="B1">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c s="2" r="C1"/>
     </row>
     <row r="2">
       <c t="s" s="2" r="A2">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c t="s" s="2" r="B2">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c s="2" r="C2"/>
     </row>
     <row r="3">
       <c t="s" s="2" r="A3">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -880,10 +972,10 @@
     </row>
     <row r="4">
       <c t="s" r="A4">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c t="s" r="B4">
-        <v>72</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Fixing more bugs with select others
</commit_message>
<xml_diff>
--- a/form-files/selects/selects.xlsx
+++ b/form-files/selects/selects.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="86" count="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="94" count="120">
   <si>
     <t>comments</t>
   </si>
@@ -25,6 +25,9 @@
     <t>appearance</t>
   </si>
   <si>
+    <t>inputAttributes.data-type</t>
+  </si>
+  <si>
     <t>condition</t>
   </si>
   <si>
@@ -125,6 +128,24 @@
   </si>
   <si>
     <t>Teal is a good choice.</t>
+  </si>
+  <si>
+    <t>horizontal</t>
+  </si>
+  <si>
+    <t>h_select</t>
+  </si>
+  <si>
+    <t>Horizontal select example.</t>
+  </si>
+  <si>
+    <t>select_one content_provider_test</t>
+  </si>
+  <si>
+    <t>cp_test</t>
+  </si>
+  <si>
+    <t>This demos a content provider query.</t>
   </si>
   <si>
     <t>list_name</t>
@@ -250,10 +271,13 @@
     <t>"https://query.yahooapis.com/v1/public/yql?format=json&amp;q=" +  encodeURIComponent("select * from geo.states where place='" + data('state') + "'")</t>
   </si>
   <si>
-    <t>odk_values</t>
+    <t>content_provider_test</t>
   </si>
   <si>
     <t>"content://com.opendatakit.tables.ContentProvider/database_id/table_id/row_id"</t>
+  </si>
+  <si>
+    <t>[{ name: "test", label : JSON.stringify(context) }]</t>
   </si>
   <si>
     <t>setting</t>
@@ -487,9 +511,10 @@
   <cols>
     <col max="1" min="1" customWidth="1" width="34.29"/>
     <col max="2" min="2" customWidth="1" width="35.0"/>
-    <col max="4" min="4" customWidth="1" width="38.71"/>
-    <col max="5" min="5" customWidth="1" width="32.71"/>
-    <col max="6" min="6" customWidth="1" width="37.71"/>
+    <col max="4" min="4" customWidth="1" width="20.71"/>
+    <col max="5" min="5" customWidth="1" width="38.71"/>
+    <col max="6" min="6" customWidth="1" width="32.71"/>
+    <col max="7" min="7" customWidth="1" width="46.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -511,174 +536,198 @@
       <c t="s" r="F1">
         <v>5</v>
       </c>
+      <c t="s" r="G1">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c t="s" s="12" r="A2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c t="s" r="B2">
-        <v>7</v>
-      </c>
-      <c t="s" r="E2">
         <v>8</v>
       </c>
       <c t="s" r="F2">
         <v>9</v>
+      </c>
+      <c t="s" r="G2">
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c s="12" r="A3"/>
       <c t="s" r="B3">
-        <v>10</v>
-      </c>
-      <c t="s" r="E3">
         <v>11</v>
       </c>
       <c t="s" r="F3">
         <v>12</v>
       </c>
+      <c t="s" r="G3">
+        <v>13</v>
+      </c>
     </row>
     <row r="4">
       <c t="s" s="12" r="A4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c t="s" r="B4">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c s="12" r="A5"/>
       <c t="s" r="B5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c t="s" r="C5">
-        <v>16</v>
-      </c>
-      <c t="s" r="E5">
         <v>17</v>
       </c>
       <c t="s" r="F5">
         <v>18</v>
+      </c>
+      <c t="s" r="G5">
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c s="12" r="A6"/>
       <c t="s" r="B6">
-        <v>19</v>
-      </c>
-      <c t="s" r="D6">
         <v>20</v>
       </c>
-      <c t="s" r="F6">
+      <c t="s" r="E6">
         <v>21</v>
+      </c>
+      <c t="s" r="G6">
+        <v>22</v>
       </c>
     </row>
     <row r="7">
       <c s="12" r="A7"/>
       <c t="s" r="B7">
-        <v>19</v>
-      </c>
-      <c t="s" r="D7">
-        <v>22</v>
-      </c>
-      <c t="s" r="F7">
+        <v>20</v>
+      </c>
+      <c t="s" r="E7">
         <v>23</v>
+      </c>
+      <c t="s" r="G7">
+        <v>24</v>
       </c>
     </row>
     <row r="8">
       <c s="12" r="A8"/>
       <c t="s" r="B8">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9">
       <c s="12" r="A9"/>
       <c t="s" r="B9">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10">
       <c s="12" r="A10"/>
       <c t="s" r="B10">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c t="s" r="C10">
-        <v>26</v>
-      </c>
-      <c t="s" r="E10">
         <v>27</v>
       </c>
       <c t="s" r="F10">
         <v>28</v>
+      </c>
+      <c t="s" r="G10">
+        <v>29</v>
       </c>
     </row>
     <row r="11">
       <c s="12" r="A11"/>
       <c t="s" r="B11">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c t="s" r="C11">
-        <v>26</v>
-      </c>
-      <c t="s" r="E11">
+        <v>27</v>
+      </c>
+      <c t="s" r="F11">
+        <v>30</v>
+      </c>
+      <c t="s" r="G11">
         <v>29</v>
-      </c>
-      <c t="s" r="F11">
-        <v>28</v>
       </c>
     </row>
     <row r="12">
       <c s="12" r="A12"/>
       <c t="s" r="B12">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c t="s" r="C12">
-        <v>26</v>
-      </c>
-      <c t="s" r="E12">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c t="s" r="F12">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c t="s" r="G12">
+        <v>29</v>
       </c>
     </row>
     <row r="13">
       <c s="12" r="A13"/>
       <c t="s" r="B13">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14">
       <c s="12" r="A14"/>
       <c t="s" r="B14">
-        <v>31</v>
-      </c>
-      <c t="s" r="E14">
         <v>32</v>
       </c>
       <c t="s" r="F14">
         <v>33</v>
       </c>
+      <c t="s" r="G14">
+        <v>34</v>
+      </c>
     </row>
     <row r="15">
       <c t="s" s="12" r="A15">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c t="s" r="B15">
-        <v>19</v>
-      </c>
-      <c t="s" r="D15">
-        <v>35</v>
-      </c>
-      <c t="s" r="F15">
+        <v>20</v>
+      </c>
+      <c t="s" r="E15">
         <v>36</v>
+      </c>
+      <c t="s" r="G15">
+        <v>37</v>
       </c>
     </row>
     <row r="16">
       <c s="12" r="A16"/>
+      <c t="s" r="B16">
+        <v>26</v>
+      </c>
+      <c t="s" r="D16">
+        <v>38</v>
+      </c>
+      <c t="s" r="F16">
+        <v>39</v>
+      </c>
+      <c t="s" r="G16">
+        <v>40</v>
+      </c>
     </row>
     <row r="17">
       <c s="12" r="A17"/>
+      <c t="s" r="B17">
+        <v>41</v>
+      </c>
+      <c t="s" r="F17">
+        <v>42</v>
+      </c>
+      <c t="s" r="G17">
+        <v>43</v>
+      </c>
     </row>
     <row r="18">
       <c s="12" r="A18"/>
@@ -711,170 +760,170 @@
   <sheetData>
     <row r="1">
       <c t="s" r="A1">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c t="s" r="B1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c t="s" r="C1">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c t="s" r="D1">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2">
       <c t="s" r="A2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c t="s" r="B2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c t="s" r="C2">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
       <c t="s" r="A3">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c t="s" r="B3">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c t="s" r="C3">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
       <c t="s" r="A4">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c t="s" r="B4">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c t="s" r="C4">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
       <c t="s" r="A5">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c t="s" r="B5">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c t="s" r="C5">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6">
       <c t="s" r="A6">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c t="s" r="B6">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c t="s" r="C6">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7">
       <c t="s" r="A7">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c t="s" r="B7">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c t="s" r="C7">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8">
       <c t="s" r="A8">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c t="s" r="B8">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c t="s" r="C8">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9">
       <c t="s" r="A9">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c t="s" r="B9">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c t="s" r="C9">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10">
       <c t="s" r="A10">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c t="s" r="B10">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c t="s" r="C10">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12">
       <c t="s" r="A12">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c t="s" r="B12">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c t="s" r="D12">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13">
       <c t="s" r="A13">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c t="s" r="B13">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c t="s" r="D13">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15">
       <c t="s" r="A15">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c t="s" r="B15">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c t="s" r="D15">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16">
       <c t="s" r="A16">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c t="s" r="B16">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c t="s" r="D16">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17">
       <c t="s" r="A17">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c t="s" r="B17">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c t="s" r="D17">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -894,43 +943,46 @@
   <sheetData>
     <row r="1">
       <c t="s" r="A1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c t="s" r="B1">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c t="s" r="C1">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2">
       <c t="s" r="A2">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c t="s" r="B2">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c t="s" r="C2">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3">
       <c t="s" r="A3">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c t="s" r="B3">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c t="s" r="C3">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5">
       <c t="s" r="A5">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c t="s" r="B5">
-        <v>78</v>
+        <v>85</v>
+      </c>
+      <c t="s" r="C5">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -946,25 +998,25 @@
   <sheetData>
     <row r="1">
       <c t="s" s="2" r="A1">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c t="s" s="2" r="B1">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c s="2" r="C1"/>
     </row>
     <row r="2">
       <c t="s" s="2" r="A2">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c t="s" s="2" r="B2">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c s="2" r="C2"/>
     </row>
     <row r="3">
       <c t="s" s="2" r="A3">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -972,10 +1024,10 @@
     </row>
     <row r="4">
       <c t="s" r="A4">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c t="s" r="B4">
-        <v>85</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Fixing name bugs in select example form
</commit_message>
<xml_diff>
--- a/form-files/selects/selects.xlsx
+++ b/form-files/selects/selects.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="108">
   <si>
     <t>comments</t>
   </si>
@@ -46,6 +46,15 @@
     <t>Cascading select using remote data</t>
   </si>
   <si>
+    <t>select_one countries</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Choose a country:</t>
+  </si>
+  <si>
     <t>select_one states</t>
   </si>
   <si>
@@ -55,15 +64,6 @@
     <t>Choose a state:</t>
   </si>
   <si>
-    <t>select_one cities</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>Choose a city:</t>
-  </si>
-  <si>
     <t>Image based select</t>
   </si>
   <si>
@@ -160,12 +160,6 @@
     <t>dropdown</t>
   </si>
   <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>Choose a country:</t>
-  </si>
-  <si>
     <t>context.region === data('region')</t>
   </si>
   <si>
@@ -286,7 +280,7 @@
     <t>callback</t>
   </si>
   <si>
-    <t>states</t>
+    <t>countries</t>
   </si>
   <si>
     <t>"https://query.yahooapis.com/v1/public/yql?format=json&amp;q=" +  encodeURIComponent("select * from geo.countries where place='North America'")</t>
@@ -298,10 +292,10 @@
 }) : []</t>
   </si>
   <si>
-    <t>cities</t>
-  </si>
-  <si>
-    <t>"https://query.yahooapis.com/v1/public/yql?format=json&amp;q=" +  encodeURIComponent("select * from geo.states where place='" + data('state') + "'")</t>
+    <t>states</t>
+  </si>
+  <si>
+    <t>"https://query.yahooapis.com/v1/public/yql?format=json&amp;q=" +  encodeURIComponent("select * from geo.states where place='" + data('country') + "'")</t>
   </si>
   <si>
     <t>regions_csv</t>
@@ -799,28 +793,28 @@
         <v>47</v>
       </c>
       <c t="s" r="F18">
+        <v>11</v>
+      </c>
+      <c t="s" r="G18">
+        <v>12</v>
+      </c>
+      <c t="s" r="I18">
         <v>48</v>
-      </c>
-      <c t="s" r="G18">
-        <v>49</v>
-      </c>
-      <c t="s" r="I18">
-        <v>50</v>
       </c>
     </row>
     <row r="19">
       <c s="12" r="A19"/>
       <c t="s" r="B19">
+        <v>49</v>
+      </c>
+      <c t="s" r="F19">
+        <v>50</v>
+      </c>
+      <c t="s" r="G19">
         <v>51</v>
       </c>
-      <c t="s" r="F19">
+      <c t="s" r="H19">
         <v>52</v>
-      </c>
-      <c t="s" r="G19">
-        <v>53</v>
-      </c>
-      <c t="s" r="H19">
-        <v>54</v>
       </c>
     </row>
     <row r="20">
@@ -854,13 +848,13 @@
   <sheetData>
     <row r="1">
       <c t="s" r="A1">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c t="s" r="B1">
         <v>5</v>
       </c>
       <c t="s" r="C1">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c t="s" r="D1">
         <v>6</v>
@@ -868,156 +862,156 @@
     </row>
     <row r="2">
       <c t="s" r="A2">
+        <v>55</v>
+      </c>
+      <c t="s" r="B2">
+        <v>56</v>
+      </c>
+      <c t="s" r="C2">
         <v>57</v>
-      </c>
-      <c t="s" r="B2">
-        <v>58</v>
-      </c>
-      <c t="s" r="C2">
-        <v>59</v>
       </c>
     </row>
     <row r="3">
       <c t="s" r="A3">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c t="s" r="B3">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c t="s" r="C3">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4">
       <c t="s" r="A4">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c t="s" r="B4">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c t="s" r="C4">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5">
       <c t="s" r="A5">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c t="s" r="B5">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c t="s" r="C5">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6">
       <c t="s" r="A6">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c t="s" r="B6">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c t="s" r="C6">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7">
       <c t="s" r="A7">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c t="s" r="B7">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c t="s" r="C7">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8">
       <c t="s" r="A8">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c t="s" r="B8">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c t="s" r="C8">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9">
       <c t="s" r="A9">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c t="s" r="B9">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c t="s" r="C9">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10">
       <c t="s" r="A10">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c t="s" r="B10">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c t="s" r="C10">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12">
       <c t="s" r="A12">
+        <v>74</v>
+      </c>
+      <c t="s" r="B12">
+        <v>75</v>
+      </c>
+      <c t="s" r="D12">
         <v>76</v>
-      </c>
-      <c t="s" r="B12">
-        <v>77</v>
-      </c>
-      <c t="s" r="D12">
-        <v>78</v>
       </c>
     </row>
     <row r="13">
       <c t="s" r="A13">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c t="s" r="B13">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c t="s" r="D13">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15">
       <c t="s" r="A15">
+        <v>79</v>
+      </c>
+      <c t="s" r="B15">
+        <v>80</v>
+      </c>
+      <c t="s" r="D15">
         <v>81</v>
-      </c>
-      <c t="s" r="B15">
-        <v>82</v>
-      </c>
-      <c t="s" r="D15">
-        <v>83</v>
       </c>
     </row>
     <row r="16">
       <c t="s" r="A16">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c t="s" r="B16">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c t="s" r="D16">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17">
       <c t="s" r="A17">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c t="s" r="B17">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c t="s" r="D17">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1040,65 +1034,65 @@
         <v>5</v>
       </c>
       <c t="s" r="B1">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c t="s" r="C1">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2">
       <c t="s" r="A2">
+        <v>88</v>
+      </c>
+      <c t="s" r="B2">
+        <v>89</v>
+      </c>
+      <c t="s" r="C2">
         <v>90</v>
-      </c>
-      <c t="s" r="B2">
-        <v>91</v>
-      </c>
-      <c t="s" r="C2">
-        <v>92</v>
       </c>
     </row>
     <row r="3">
       <c t="s" r="A3">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c t="s" r="B3">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c t="s" r="C3">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4">
       <c t="s" r="A4">
+        <v>93</v>
+      </c>
+      <c t="s" r="B4">
+        <v>94</v>
+      </c>
+      <c t="s" r="C4">
         <v>95</v>
-      </c>
-      <c t="s" r="B4">
-        <v>96</v>
-      </c>
-      <c t="s" r="C4">
-        <v>97</v>
       </c>
     </row>
     <row r="5">
       <c t="s" r="A5">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c t="s" r="B5">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c t="s" r="C5">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6">
       <c t="s" r="A6">
+        <v>98</v>
+      </c>
+      <c t="s" r="B6">
+        <v>99</v>
+      </c>
+      <c t="s" r="C6">
         <v>100</v>
-      </c>
-      <c t="s" r="B6">
-        <v>101</v>
-      </c>
-      <c t="s" r="C6">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1114,25 +1108,25 @@
   <sheetData>
     <row r="1">
       <c t="s" s="2" r="A1">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c t="s" s="2" r="B1">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c s="2" r="C1"/>
     </row>
     <row r="2">
       <c t="s" s="2" r="A2">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c t="s" s="2" r="B2">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c s="2" r="C2"/>
     </row>
     <row r="3">
       <c t="s" s="2" r="A3">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1140,10 +1134,10 @@
     </row>
     <row r="4">
       <c t="s" r="A4">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c t="s" r="B4">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6">

</xml_diff>